<commit_message>
enum value related bug fixed
</commit_message>
<xml_diff>
--- a/Data Dictionary.xlsx
+++ b/Data Dictionary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zahab\Desktop\xampp\htdocs\Patient\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9A329AFF-002B-4340-AAD5-6CC2A80BB759}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{243AACD2-C375-4815-80E9-EDBC642153D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{26241A9F-144A-46DD-AB7A-6DA5F468646E}"/>
   </bookViews>
@@ -124,9 +124,6 @@
     <t>age_type</t>
   </si>
   <si>
-    <t>VARCHAR(10)</t>
-  </si>
-  <si>
     <t>Unit for age (e.g., Years, Months)</t>
   </si>
   <si>
@@ -245,6 +242,9 @@
   </si>
   <si>
     <t>Foreign key referencing presentfacility(id)</t>
+  </si>
+  <si>
+    <t>ENUM('Years', 'Months')</t>
   </si>
 </sst>
 </file>
@@ -653,8 +653,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E0BAA0D-0C2D-4D91-804E-27E5351A5607}">
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -690,7 +690,7 @@
         <v>6</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
@@ -808,10 +808,10 @@
         <v>27</v>
       </c>
       <c r="B11" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>29</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>10</v>
@@ -819,13 +819,13 @@
     </row>
     <row r="12" spans="1:4" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="C12" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>32</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>10</v>
@@ -833,25 +833,25 @@
     </row>
     <row r="13" spans="1:4" ht="31" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="C13" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="D13" s="2"/>
+    </row>
+    <row r="14" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A14" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D13" s="2"/>
-    </row>
-    <row r="14" spans="1:4" ht="31" x14ac:dyDescent="0.35">
-      <c r="A14" s="2" t="s">
+      <c r="B14" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="C14" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>38</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>10</v>
@@ -859,25 +859,25 @@
     </row>
     <row r="15" spans="1:4" ht="31" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D15" s="2"/>
     </row>
     <row r="16" spans="1:4" ht="31" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D16" s="2"/>
     </row>
@@ -925,81 +925,81 @@
         <v>5</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="31" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>42</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>43</v>
       </c>
       <c r="D3" s="2"/>
     </row>
     <row r="4" spans="1:4" ht="31" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>44</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>45</v>
       </c>
       <c r="D4" s="2"/>
     </row>
     <row r="5" spans="1:4" ht="31" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>46</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>47</v>
       </c>
       <c r="D5" s="2"/>
     </row>
     <row r="6" spans="1:4" ht="31" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D6" s="2"/>
     </row>
     <row r="7" spans="1:4" ht="31" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="C7" s="2" t="s">
         <v>51</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>52</v>
       </c>
       <c r="D7" s="2"/>
     </row>
     <row r="8" spans="1:4" ht="31" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D8" s="2"/>
     </row>
@@ -1047,69 +1047,69 @@
         <v>5</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="31" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>56</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>57</v>
       </c>
       <c r="D3" s="2"/>
     </row>
     <row r="4" spans="1:4" ht="31" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>58</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>59</v>
       </c>
       <c r="D4" s="2"/>
     </row>
     <row r="5" spans="1:4" ht="31" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>60</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>61</v>
       </c>
       <c r="D5" s="2"/>
     </row>
     <row r="6" spans="1:4" ht="31" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>62</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>63</v>
       </c>
       <c r="D6" s="2"/>
     </row>
     <row r="7" spans="1:4" ht="31" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D7" s="2"/>
     </row>

</xml_diff>